<commit_message>
added Hull-White calibration of a and sigma parameters
</commit_message>
<xml_diff>
--- a/Hull-white model/sample_data.xlsx
+++ b/Hull-white model/sample_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hw_data_monthly" sheetId="18" r:id="rId1"/>
@@ -17,12 +17,14 @@
     <sheet name="zero_bond_dates" sheetId="15" r:id="rId3"/>
     <sheet name="bond_dates" sheetId="10" r:id="rId4"/>
     <sheet name="payment_dates" sheetId="17" r:id="rId5"/>
-    <sheet name="european_exercise_dates" sheetId="16" r:id="rId6"/>
-    <sheet name="bermudan_exercise_dates" sheetId="11" r:id="rId7"/>
-    <sheet name="callable_exercise_dates" sheetId="13" r:id="rId8"/>
+    <sheet name="caplet_dates" sheetId="19" r:id="rId6"/>
+    <sheet name="european_exercise_dates" sheetId="16" r:id="rId7"/>
+    <sheet name="bermudan_exercise_dates" sheetId="11" r:id="rId8"/>
+    <sheet name="callable_exercise_dates" sheetId="13" r:id="rId9"/>
+    <sheet name="callable_payment_dates" sheetId="20" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="K">[1]d!$B$26</definedName>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
   <si>
     <t>ZCB</t>
   </si>
@@ -68,6 +70,12 @@
   </si>
   <si>
     <t>Step</t>
+  </si>
+  <si>
+    <t>Reset Date</t>
+  </si>
+  <si>
+    <t>Reset Step</t>
   </si>
 </sst>
 </file>
@@ -706,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1225C002-4F43-4A7E-AE36-BA9B5839E624}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,6 +1404,156 @@
       </c>
       <c r="C62" s="11">
         <v>0.94204293185247345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4AF90A-030D-4DBE-B558-20C772CE556C}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>43188</v>
+      </c>
+      <c r="B2" s="2">
+        <f>+VLOOKUP(A2,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.3122450511295989E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>43372</v>
+      </c>
+      <c r="B3" s="2">
+        <f>+VLOOKUP(A3,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1.3122450511295989E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>43553</v>
+      </c>
+      <c r="B4" s="2">
+        <f>+VLOOKUP(A4,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43737</v>
+      </c>
+      <c r="B5" s="2">
+        <f>+VLOOKUP(A5,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>24</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43919</v>
+      </c>
+      <c r="B6" s="2">
+        <f>+VLOOKUP(A6,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>30</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>44103</v>
+      </c>
+      <c r="B7" s="2">
+        <f>+VLOOKUP(A7,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>36</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>44284</v>
+      </c>
+      <c r="B8" s="2">
+        <f>+VLOOKUP(A8,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>42</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>44468</v>
+      </c>
+      <c r="B9" s="2">
+        <f>+VLOOKUP(A9,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>48</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>44649</v>
+      </c>
+      <c r="B10" s="2">
+        <f>+VLOOKUP(A10,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>54</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.3122450511295999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44833</v>
+      </c>
+      <c r="B11" s="2">
+        <f>+VLOOKUP(A11,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>60</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1.3122450511295999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2171,7 +2329,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,6 +2603,54 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4EEAD1-57EB-489B-855B-D4EA02E343E7}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>43188</v>
+      </c>
+      <c r="B2" s="2">
+        <f>+VLOOKUP(A2,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43098</v>
+      </c>
+      <c r="D2" s="2">
+        <f>+VLOOKUP(C2,tree_dates!$A$2:$B$62,2,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596B4464-469A-43D7-97B6-1D122B71C9F7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2478,7 +2684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3857A477-F0D3-469D-8BB0-DA97E56654D7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2550,12 +2756,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F654086-DC6F-41FB-A9FC-32D893112BE1}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>